<commit_message>
Refactor code structure for improved readability and maintainability Added README file
</commit_message>
<xml_diff>
--- a/exercise_1_etl_pipeline/data/relaciones.xlsx
+++ b/exercise_1_etl_pipeline/data/relaciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugen\Desktop\Palace\the-palace-company-challenge\exercise_1_etl_pipeline\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diani\Dropbox\1 TESIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0817E6-4BEC-4F60-8677-78B8C45D64E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC2D9E4-00E1-40C4-8CAD-4885B247E882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz de adyacencia" sheetId="1" r:id="rId1"/>
@@ -433,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -447,18 +447,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -742,13 +753,13 @@
   <dimension ref="A1:AZ52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
   </cols>
@@ -982,10 +993,10 @@
       <c r="AA2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AB2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AC2" s="9" t="s">
         <v>25</v>
       </c>
       <c r="AD2" s="1" t="s">
@@ -1065,154 +1076,154 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6">
-        <v>1</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0</v>
-      </c>
-      <c r="K3" s="8">
-        <v>0</v>
-      </c>
-      <c r="L3" s="6">
-        <v>1</v>
-      </c>
-      <c r="M3" s="8">
-        <v>0</v>
-      </c>
-      <c r="N3" s="8">
-        <v>0</v>
-      </c>
-      <c r="O3" s="8">
-        <v>0</v>
-      </c>
-      <c r="P3" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="8">
-        <v>0</v>
-      </c>
-      <c r="R3" s="8">
-        <v>0</v>
-      </c>
-      <c r="S3" s="8">
-        <v>0</v>
-      </c>
-      <c r="T3" s="8">
-        <v>0</v>
-      </c>
-      <c r="U3" s="8">
-        <v>0</v>
-      </c>
-      <c r="V3" s="8">
-        <v>0</v>
-      </c>
-      <c r="W3" s="9">
-        <v>0</v>
-      </c>
-      <c r="X3" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="6">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AH3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AI3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AJ3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AL3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AT3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AU3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AV3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AW3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AX3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AY3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AZ3" s="3">
+      <c r="C3" s="15">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0</v>
+      </c>
+      <c r="J3" s="10">
+        <v>0</v>
+      </c>
+      <c r="K3" s="10">
+        <v>0</v>
+      </c>
+      <c r="L3" s="7">
+        <v>1</v>
+      </c>
+      <c r="M3" s="10">
+        <v>0</v>
+      </c>
+      <c r="N3" s="10">
+        <v>0</v>
+      </c>
+      <c r="O3" s="10">
+        <v>0</v>
+      </c>
+      <c r="P3" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>0</v>
+      </c>
+      <c r="R3" s="10">
+        <v>0</v>
+      </c>
+      <c r="S3" s="10">
+        <v>0</v>
+      </c>
+      <c r="T3" s="10">
+        <v>0</v>
+      </c>
+      <c r="U3" s="10">
+        <v>0</v>
+      </c>
+      <c r="V3" s="10">
+        <v>0</v>
+      </c>
+      <c r="W3" s="11">
+        <v>0</v>
+      </c>
+      <c r="X3" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="12">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="13">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="13">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="13">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="13">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="13">
+        <v>1</v>
+      </c>
+      <c r="AL3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AW3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AX3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AY3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AZ3" s="13">
         <v>0</v>
       </c>
     </row>
@@ -1226,7 +1237,7 @@
       <c r="C4" s="6">
         <v>0</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="15">
         <v>0</v>
       </c>
       <c r="E4" s="6">
@@ -1283,7 +1294,7 @@
       <c r="V4" s="3">
         <v>0</v>
       </c>
-      <c r="W4" s="7">
+      <c r="W4" s="8">
         <v>0</v>
       </c>
       <c r="X4" s="3">
@@ -1387,7 +1398,7 @@
       <c r="D5" s="6">
         <v>0</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="15">
         <v>0</v>
       </c>
       <c r="F5" s="6">
@@ -1441,7 +1452,7 @@
       <c r="V5" s="3">
         <v>0</v>
       </c>
-      <c r="W5" s="7">
+      <c r="W5" s="8">
         <v>0</v>
       </c>
       <c r="X5" s="3">
@@ -1548,7 +1559,7 @@
       <c r="E6" s="6">
         <v>1</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="15">
         <v>0</v>
       </c>
       <c r="G6" s="6">
@@ -1599,7 +1610,7 @@
       <c r="V6" s="3">
         <v>0</v>
       </c>
-      <c r="W6" s="7">
+      <c r="W6" s="8">
         <v>0</v>
       </c>
       <c r="X6" s="3">
@@ -1709,7 +1720,7 @@
       <c r="F7" s="6">
         <v>1</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="15">
         <v>0</v>
       </c>
       <c r="H7" s="6">
@@ -1757,7 +1768,7 @@
       <c r="V7" s="3">
         <v>0</v>
       </c>
-      <c r="W7" s="7">
+      <c r="W7" s="8">
         <v>0</v>
       </c>
       <c r="X7" s="3">
@@ -1870,7 +1881,7 @@
       <c r="G8" s="6">
         <v>1</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="15">
         <v>0</v>
       </c>
       <c r="I8" s="6">
@@ -1915,7 +1926,7 @@
       <c r="V8" s="3">
         <v>0</v>
       </c>
-      <c r="W8" s="7">
+      <c r="W8" s="8">
         <v>0</v>
       </c>
       <c r="X8" s="3">
@@ -2031,7 +2042,7 @@
       <c r="H9" s="6">
         <v>1</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="15">
         <v>0</v>
       </c>
       <c r="J9" s="3">
@@ -2073,7 +2084,7 @@
       <c r="V9" s="3">
         <v>0</v>
       </c>
-      <c r="W9" s="7">
+      <c r="W9" s="8">
         <v>0</v>
       </c>
       <c r="X9" s="3">
@@ -2192,7 +2203,7 @@
       <c r="I10" s="3">
         <v>1</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="15">
         <v>0</v>
       </c>
       <c r="K10" s="3">
@@ -2231,7 +2242,7 @@
       <c r="V10" s="3">
         <v>0</v>
       </c>
-      <c r="W10" s="7">
+      <c r="W10" s="8">
         <v>0</v>
       </c>
       <c r="X10" s="3">
@@ -2353,7 +2364,7 @@
       <c r="J11" s="3">
         <v>1</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="15">
         <v>0</v>
       </c>
       <c r="L11" s="3">
@@ -2389,7 +2400,7 @@
       <c r="V11" s="3">
         <v>0</v>
       </c>
-      <c r="W11" s="7">
+      <c r="W11" s="8">
         <v>0</v>
       </c>
       <c r="X11" s="3">
@@ -2514,7 +2525,7 @@
       <c r="K12" s="3">
         <v>1</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="15">
         <v>0</v>
       </c>
       <c r="M12" s="3">
@@ -2547,7 +2558,7 @@
       <c r="V12" s="3">
         <v>0</v>
       </c>
-      <c r="W12" s="7">
+      <c r="W12" s="8">
         <v>0</v>
       </c>
       <c r="X12" s="3">
@@ -2675,7 +2686,7 @@
       <c r="L13" s="3">
         <v>1</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="15">
         <v>0</v>
       </c>
       <c r="N13" s="3">
@@ -2705,7 +2716,7 @@
       <c r="V13" s="3">
         <v>0</v>
       </c>
-      <c r="W13" s="7">
+      <c r="W13" s="8">
         <v>0</v>
       </c>
       <c r="X13" s="3">
@@ -2836,7 +2847,7 @@
       <c r="M14" s="3">
         <v>1</v>
       </c>
-      <c r="N14" s="11">
+      <c r="N14" s="15">
         <v>0</v>
       </c>
       <c r="O14" s="3">
@@ -2863,7 +2874,7 @@
       <c r="V14" s="3">
         <v>0</v>
       </c>
-      <c r="W14" s="7">
+      <c r="W14" s="8">
         <v>0</v>
       </c>
       <c r="X14" s="3">
@@ -2997,7 +3008,7 @@
       <c r="N15" s="3">
         <v>0</v>
       </c>
-      <c r="O15" s="11">
+      <c r="O15" s="15">
         <v>0</v>
       </c>
       <c r="P15" s="3">
@@ -3021,7 +3032,7 @@
       <c r="V15" s="3">
         <v>0</v>
       </c>
-      <c r="W15" s="7">
+      <c r="W15" s="8">
         <v>0</v>
       </c>
       <c r="X15" s="3">
@@ -3158,7 +3169,7 @@
       <c r="O16" s="3">
         <v>1</v>
       </c>
-      <c r="P16" s="11">
+      <c r="P16" s="15">
         <v>0</v>
       </c>
       <c r="Q16" s="3">
@@ -3179,7 +3190,7 @@
       <c r="V16" s="3">
         <v>0</v>
       </c>
-      <c r="W16" s="7">
+      <c r="W16" s="8">
         <v>0</v>
       </c>
       <c r="X16" s="3">
@@ -3319,7 +3330,7 @@
       <c r="P17" s="3">
         <v>1</v>
       </c>
-      <c r="Q17" s="11">
+      <c r="Q17" s="15">
         <v>0</v>
       </c>
       <c r="R17" s="3">
@@ -3337,7 +3348,7 @@
       <c r="V17" s="3">
         <v>0</v>
       </c>
-      <c r="W17" s="7">
+      <c r="W17" s="8">
         <v>0</v>
       </c>
       <c r="X17" s="3">
@@ -3480,7 +3491,7 @@
       <c r="Q18" s="3">
         <v>1</v>
       </c>
-      <c r="R18" s="11">
+      <c r="R18" s="15">
         <v>0</v>
       </c>
       <c r="S18" s="3">
@@ -3495,7 +3506,7 @@
       <c r="V18" s="3">
         <v>1</v>
       </c>
-      <c r="W18" s="7">
+      <c r="W18" s="8">
         <v>1</v>
       </c>
       <c r="X18" s="3">
@@ -3641,7 +3652,7 @@
       <c r="R19" s="3">
         <v>1</v>
       </c>
-      <c r="S19" s="11">
+      <c r="S19" s="15">
         <v>0</v>
       </c>
       <c r="T19" s="3">
@@ -3653,7 +3664,7 @@
       <c r="V19" s="3">
         <v>1</v>
       </c>
-      <c r="W19" s="7">
+      <c r="W19" s="8">
         <v>1</v>
       </c>
       <c r="X19" s="3">
@@ -3751,156 +3762,58 @@
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="3">
-        <v>1</v>
-      </c>
-      <c r="D20" s="3">
-        <v>0</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0</v>
-      </c>
-      <c r="G20" s="3">
-        <v>0</v>
-      </c>
-      <c r="H20" s="3">
-        <v>0</v>
-      </c>
-      <c r="I20" s="3">
-        <v>0</v>
-      </c>
-      <c r="J20" s="3">
-        <v>0</v>
-      </c>
-      <c r="K20" s="3">
-        <v>0</v>
-      </c>
-      <c r="L20" s="3">
-        <v>0</v>
-      </c>
-      <c r="M20" s="3">
-        <v>0</v>
-      </c>
-      <c r="N20" s="3">
-        <v>0</v>
-      </c>
-      <c r="O20" s="3">
-        <v>0</v>
-      </c>
-      <c r="P20" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="3">
-        <v>0</v>
-      </c>
-      <c r="R20" s="3">
-        <v>0</v>
-      </c>
-      <c r="S20" s="3">
-        <v>1</v>
-      </c>
-      <c r="T20" s="11">
-        <v>0</v>
-      </c>
-      <c r="U20" s="3">
-        <v>0</v>
-      </c>
-      <c r="V20" s="3">
-        <v>0</v>
-      </c>
-      <c r="W20" s="7">
-        <v>0</v>
-      </c>
-      <c r="X20" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AJ20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AK20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AN20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AO20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AP20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AQ20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AR20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AS20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AT20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AU20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AV20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AW20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AX20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AY20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AZ20" s="3">
-        <v>0</v>
-      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="15">
+        <v>0</v>
+      </c>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="3"/>
+      <c r="AC20" s="3"/>
+      <c r="AD20" s="3"/>
+      <c r="AE20" s="3"/>
+      <c r="AF20" s="3"/>
+      <c r="AG20" s="3"/>
+      <c r="AH20" s="3"/>
+      <c r="AI20" s="3"/>
+      <c r="AJ20" s="3"/>
+      <c r="AK20" s="3"/>
+      <c r="AL20" s="3"/>
+      <c r="AM20" s="3"/>
+      <c r="AN20" s="3"/>
+      <c r="AO20" s="3"/>
+      <c r="AP20" s="3"/>
+      <c r="AQ20" s="3"/>
+      <c r="AR20" s="3"/>
+      <c r="AS20" s="3"/>
+      <c r="AT20" s="3"/>
+      <c r="AU20" s="3"/>
+      <c r="AV20" s="3"/>
+      <c r="AW20" s="3"/>
+      <c r="AX20" s="3"/>
+      <c r="AY20" s="3"/>
+      <c r="AZ20" s="3"/>
     </row>
     <row r="21" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
@@ -3927,11 +3840,11 @@
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
-      <c r="U21" s="11">
+      <c r="U21" s="15">
         <v>0</v>
       </c>
       <c r="V21" s="3"/>
-      <c r="W21" s="7"/>
+      <c r="W21" s="8"/>
       <c r="X21" s="3"/>
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
@@ -3988,10 +3901,10 @@
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
-      <c r="V22" s="11">
-        <v>0</v>
-      </c>
-      <c r="W22" s="7"/>
+      <c r="V22" s="15">
+        <v>0</v>
+      </c>
+      <c r="W22" s="8"/>
       <c r="X22" s="3"/>
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
@@ -4049,7 +3962,7 @@
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
-      <c r="W23" s="11">
+      <c r="W23" s="15">
         <v>0</v>
       </c>
       <c r="X23" s="3"/>
@@ -4109,8 +4022,8 @@
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
-      <c r="W24" s="7"/>
-      <c r="X24" s="11">
+      <c r="W24" s="8"/>
+      <c r="X24" s="15">
         <v>0</v>
       </c>
       <c r="Y24" s="3"/>
@@ -4169,9 +4082,9 @@
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
-      <c r="W25" s="7"/>
+      <c r="W25" s="8"/>
       <c r="X25" s="3"/>
-      <c r="Y25" s="11">
+      <c r="Y25" s="15">
         <v>0</v>
       </c>
       <c r="Z25" s="3"/>
@@ -4229,10 +4142,10 @@
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
-      <c r="W26" s="7"/>
+      <c r="W26" s="8"/>
       <c r="X26" s="3"/>
       <c r="Y26" s="3"/>
-      <c r="Z26" s="11">
+      <c r="Z26" s="15">
         <v>0</v>
       </c>
       <c r="AA26" s="3"/>
@@ -4289,11 +4202,11 @@
       <c r="T27" s="3"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
-      <c r="W27" s="7"/>
+      <c r="W27" s="8"/>
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
-      <c r="AA27" s="11">
+      <c r="AA27" s="15">
         <v>0</v>
       </c>
       <c r="AB27" s="3"/>
@@ -4323,7 +4236,7 @@
       <c r="AZ27" s="3"/>
     </row>
     <row r="28" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
+      <c r="A28" s="14">
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -4349,12 +4262,12 @@
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
-      <c r="W28" s="7"/>
+      <c r="W28" s="8"/>
       <c r="X28" s="3"/>
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
       <c r="AA28" s="3"/>
-      <c r="AB28" s="11">
+      <c r="AB28" s="15">
         <v>0</v>
       </c>
       <c r="AC28" s="3"/>
@@ -4415,7 +4328,7 @@
       <c r="Z29" s="3"/>
       <c r="AA29" s="3"/>
       <c r="AB29" s="3"/>
-      <c r="AC29" s="11">
+      <c r="AC29" s="15">
         <v>0</v>
       </c>
       <c r="AD29" s="3"/>
@@ -4476,7 +4389,7 @@
       <c r="AA30" s="3"/>
       <c r="AB30" s="3"/>
       <c r="AC30" s="3"/>
-      <c r="AD30" s="11">
+      <c r="AD30" s="15">
         <v>0</v>
       </c>
       <c r="AE30" s="3"/>
@@ -4537,7 +4450,7 @@
       <c r="AB31" s="3"/>
       <c r="AC31" s="3"/>
       <c r="AD31" s="3"/>
-      <c r="AE31" s="11">
+      <c r="AE31" s="15">
         <v>0</v>
       </c>
       <c r="AF31" s="3"/>
@@ -4598,7 +4511,7 @@
       <c r="AC32" s="3"/>
       <c r="AD32" s="3"/>
       <c r="AE32" s="3"/>
-      <c r="AF32" s="11">
+      <c r="AF32" s="15">
         <v>0</v>
       </c>
       <c r="AG32" s="3"/>
@@ -4659,7 +4572,7 @@
       <c r="AD33" s="3"/>
       <c r="AE33" s="3"/>
       <c r="AF33" s="3"/>
-      <c r="AG33" s="11">
+      <c r="AG33" s="15">
         <v>0</v>
       </c>
       <c r="AH33" s="3"/>
@@ -4720,7 +4633,7 @@
       <c r="AE34" s="3"/>
       <c r="AF34" s="3"/>
       <c r="AG34" s="3"/>
-      <c r="AH34" s="11">
+      <c r="AH34" s="15">
         <v>0</v>
       </c>
       <c r="AI34" s="3"/>
@@ -4781,7 +4694,7 @@
       <c r="AF35" s="3"/>
       <c r="AG35" s="3"/>
       <c r="AH35" s="3"/>
-      <c r="AI35" s="11">
+      <c r="AI35" s="15">
         <v>0</v>
       </c>
       <c r="AJ35" s="3"/>
@@ -4842,7 +4755,7 @@
       <c r="AG36" s="3"/>
       <c r="AH36" s="3"/>
       <c r="AI36" s="3"/>
-      <c r="AJ36" s="11">
+      <c r="AJ36" s="15">
         <v>0</v>
       </c>
       <c r="AK36" s="3"/>
@@ -4903,7 +4816,7 @@
       <c r="AH37" s="3"/>
       <c r="AI37" s="3"/>
       <c r="AJ37" s="3"/>
-      <c r="AK37" s="11">
+      <c r="AK37" s="15">
         <v>0</v>
       </c>
       <c r="AL37" s="3"/>
@@ -4964,7 +4877,7 @@
       <c r="AI38" s="3"/>
       <c r="AJ38" s="3"/>
       <c r="AK38" s="3"/>
-      <c r="AL38" s="11">
+      <c r="AL38" s="15">
         <v>0</v>
       </c>
       <c r="AM38" s="3"/>
@@ -5025,7 +4938,7 @@
       <c r="AJ39" s="3"/>
       <c r="AK39" s="3"/>
       <c r="AL39" s="3"/>
-      <c r="AM39" s="11">
+      <c r="AM39" s="15">
         <v>0</v>
       </c>
       <c r="AN39" s="3"/>
@@ -5086,7 +4999,7 @@
       <c r="AK40" s="3"/>
       <c r="AL40" s="3"/>
       <c r="AM40" s="3"/>
-      <c r="AN40" s="11">
+      <c r="AN40" s="15">
         <v>0</v>
       </c>
       <c r="AO40" s="3"/>
@@ -5147,7 +5060,7 @@
       <c r="AL41" s="3"/>
       <c r="AM41" s="3"/>
       <c r="AN41" s="3"/>
-      <c r="AO41" s="11">
+      <c r="AO41" s="15">
         <v>0</v>
       </c>
       <c r="AP41" s="3"/>
@@ -5208,7 +5121,7 @@
       <c r="AM42" s="3"/>
       <c r="AN42" s="3"/>
       <c r="AO42" s="3"/>
-      <c r="AP42" s="11">
+      <c r="AP42" s="15">
         <v>0</v>
       </c>
       <c r="AQ42" s="3"/>
@@ -5269,7 +5182,7 @@
       <c r="AN43" s="3"/>
       <c r="AO43" s="3"/>
       <c r="AP43" s="3"/>
-      <c r="AQ43" s="11">
+      <c r="AQ43" s="15">
         <v>0</v>
       </c>
       <c r="AR43" s="3"/>
@@ -5330,7 +5243,7 @@
       <c r="AO44" s="3"/>
       <c r="AP44" s="3"/>
       <c r="AQ44" s="3"/>
-      <c r="AR44" s="11">
+      <c r="AR44" s="15">
         <v>0</v>
       </c>
       <c r="AS44" s="3"/>
@@ -5391,7 +5304,7 @@
       <c r="AP45" s="3"/>
       <c r="AQ45" s="3"/>
       <c r="AR45" s="3"/>
-      <c r="AS45" s="11">
+      <c r="AS45" s="15">
         <v>0</v>
       </c>
       <c r="AT45" s="3"/>
@@ -5452,7 +5365,7 @@
       <c r="AQ46" s="3"/>
       <c r="AR46" s="3"/>
       <c r="AS46" s="3"/>
-      <c r="AT46" s="11">
+      <c r="AT46" s="15">
         <v>0</v>
       </c>
       <c r="AU46" s="3"/>
@@ -5513,7 +5426,7 @@
       <c r="AR47" s="3"/>
       <c r="AS47" s="3"/>
       <c r="AT47" s="3"/>
-      <c r="AU47" s="11">
+      <c r="AU47" s="15">
         <v>0</v>
       </c>
       <c r="AV47" s="3"/>
@@ -5574,7 +5487,7 @@
       <c r="AS48" s="3"/>
       <c r="AT48" s="3"/>
       <c r="AU48" s="3"/>
-      <c r="AV48" s="11">
+      <c r="AV48" s="15">
         <v>0</v>
       </c>
       <c r="AW48" s="3"/>
@@ -5635,7 +5548,7 @@
       <c r="AT49" s="3"/>
       <c r="AU49" s="3"/>
       <c r="AV49" s="3"/>
-      <c r="AW49" s="11">
+      <c r="AW49" s="15">
         <v>0</v>
       </c>
       <c r="AX49" s="3"/>
@@ -5696,7 +5609,7 @@
       <c r="AU50" s="3"/>
       <c r="AV50" s="3"/>
       <c r="AW50" s="3"/>
-      <c r="AX50" s="11">
+      <c r="AX50" s="15">
         <v>0</v>
       </c>
       <c r="AY50" s="3"/>
@@ -5757,7 +5670,7 @@
       <c r="AV51" s="3"/>
       <c r="AW51" s="3"/>
       <c r="AX51" s="3"/>
-      <c r="AY51" s="11">
+      <c r="AY51" s="15">
         <v>0</v>
       </c>
       <c r="AZ51" s="3"/>
@@ -5818,7 +5731,7 @@
       <c r="AW52" s="3"/>
       <c r="AX52" s="3"/>
       <c r="AY52" s="3"/>
-      <c r="AZ52" s="11">
+      <c r="AZ52" s="15">
         <v>0</v>
       </c>
     </row>
@@ -5836,7 +5749,7 @@
       <selection activeCell="C21" sqref="C21:C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.140625" customWidth="1"/>
@@ -5847,7 +5760,7 @@
       <c r="B4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="16"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -5856,7 +5769,7 @@
       <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="16" t="s">
         <v>29</v>
       </c>
     </row>
@@ -5867,7 +5780,7 @@
       <c r="B6" s="3">
         <v>2</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="16" t="s">
         <v>30</v>
       </c>
     </row>
@@ -5878,7 +5791,7 @@
       <c r="B7" s="3">
         <v>3</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="16" t="s">
         <v>31</v>
       </c>
     </row>
@@ -5889,7 +5802,7 @@
       <c r="B8" s="3">
         <v>4</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="16" t="s">
         <v>32</v>
       </c>
     </row>
@@ -5900,7 +5813,7 @@
       <c r="B9" s="3">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="16" t="s">
         <v>33</v>
       </c>
     </row>
@@ -5911,7 +5824,7 @@
       <c r="B10" s="3">
         <v>6</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="16" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5922,7 +5835,7 @@
       <c r="B11" s="3">
         <v>7</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="16" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5933,7 +5846,7 @@
       <c r="B12" s="3">
         <v>8</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="16" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5944,7 +5857,7 @@
       <c r="B13" s="3">
         <v>9</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="16" t="s">
         <v>37</v>
       </c>
     </row>
@@ -5955,7 +5868,7 @@
       <c r="B14" s="3">
         <v>10</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -5966,7 +5879,7 @@
       <c r="B15" s="3">
         <v>11</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="16" t="s">
         <v>39</v>
       </c>
     </row>
@@ -5977,7 +5890,7 @@
       <c r="B16" s="3">
         <v>12</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="16" t="s">
         <v>40</v>
       </c>
     </row>
@@ -5988,7 +5901,7 @@
       <c r="B17" s="3">
         <v>13</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="16" t="s">
         <v>41</v>
       </c>
     </row>
@@ -5999,7 +5912,7 @@
       <c r="B18" s="3">
         <v>14</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="17" t="s">
         <v>42</v>
       </c>
     </row>
@@ -6010,7 +5923,7 @@
       <c r="B19" s="3">
         <v>15</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="17" t="s">
         <v>43</v>
       </c>
     </row>
@@ -6021,7 +5934,7 @@
       <c r="B20" s="3">
         <v>16</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="17" t="s">
         <v>44</v>
       </c>
     </row>
@@ -6032,7 +5945,7 @@
       <c r="B21" s="3">
         <v>17</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="17" t="s">
         <v>45</v>
       </c>
     </row>
@@ -6043,7 +5956,7 @@
       <c r="B22" s="3">
         <v>18</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="17" t="s">
         <v>46</v>
       </c>
     </row>
@@ -6054,7 +5967,7 @@
       <c r="B23" s="3">
         <v>19</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="17" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6065,7 +5978,7 @@
       <c r="B24" s="3">
         <v>20</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="17" t="s">
         <v>48</v>
       </c>
     </row>
@@ -6076,7 +5989,7 @@
       <c r="B25" s="3">
         <v>21</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="17" t="s">
         <v>49</v>
       </c>
     </row>
@@ -6087,7 +6000,7 @@
       <c r="B26" s="3">
         <v>22</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -6098,7 +6011,7 @@
       <c r="B27" s="3">
         <v>23</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="17" t="s">
         <v>51</v>
       </c>
     </row>
@@ -6109,7 +6022,7 @@
       <c r="B28" s="3">
         <v>24</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -6120,7 +6033,7 @@
       <c r="B29" s="3">
         <v>25</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="16" t="s">
         <v>53</v>
       </c>
     </row>
@@ -6131,7 +6044,7 @@
       <c r="B30" s="3">
         <v>26</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="16" t="s">
         <v>54</v>
       </c>
     </row>
@@ -6142,7 +6055,7 @@
       <c r="B31" s="3">
         <v>27</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="16" t="s">
         <v>55</v>
       </c>
     </row>
@@ -6153,7 +6066,7 @@
       <c r="B32" s="3">
         <v>28</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="16" t="s">
         <v>99</v>
       </c>
     </row>
@@ -6164,7 +6077,7 @@
       <c r="B33" s="3">
         <v>29</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="16" t="s">
         <v>56</v>
       </c>
     </row>
@@ -6175,7 +6088,7 @@
       <c r="B34" s="3">
         <v>30</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="16" t="s">
         <v>57</v>
       </c>
     </row>
@@ -6186,7 +6099,7 @@
       <c r="B35" s="3">
         <v>31</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="16" t="s">
         <v>58</v>
       </c>
     </row>
@@ -6197,7 +6110,7 @@
       <c r="B36" s="3">
         <v>32</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="16" t="s">
         <v>59</v>
       </c>
     </row>
@@ -6208,7 +6121,7 @@
       <c r="B37" s="3">
         <v>33</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="16" t="s">
         <v>60</v>
       </c>
     </row>
@@ -6219,7 +6132,7 @@
       <c r="B38" s="3">
         <v>34</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="16" t="s">
         <v>61</v>
       </c>
     </row>
@@ -6230,7 +6143,7 @@
       <c r="B39" s="3">
         <v>35</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="16" t="s">
         <v>62</v>
       </c>
     </row>
@@ -6241,7 +6154,7 @@
       <c r="B40" s="3">
         <v>36</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="16" t="s">
         <v>63</v>
       </c>
     </row>
@@ -6252,7 +6165,7 @@
       <c r="B41" s="3">
         <v>37</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="16" t="s">
         <v>64</v>
       </c>
     </row>
@@ -6263,7 +6176,7 @@
       <c r="B42" s="3">
         <v>38</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="16" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6274,7 +6187,7 @@
       <c r="B43" s="3">
         <v>39</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="16" t="s">
         <v>66</v>
       </c>
     </row>
@@ -6285,7 +6198,7 @@
       <c r="B44" s="3">
         <v>40</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="16" t="s">
         <v>67</v>
       </c>
     </row>
@@ -6296,7 +6209,7 @@
       <c r="B45" s="3">
         <v>41</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="16" t="s">
         <v>68</v>
       </c>
     </row>
@@ -6307,7 +6220,7 @@
       <c r="B46" s="3">
         <v>42</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="16" t="s">
         <v>69</v>
       </c>
     </row>
@@ -6318,7 +6231,7 @@
       <c r="B47" s="3">
         <v>43</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="16" t="s">
         <v>70</v>
       </c>
     </row>
@@ -6329,7 +6242,7 @@
       <c r="B48" s="3">
         <v>44</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="16" t="s">
         <v>71</v>
       </c>
     </row>
@@ -6340,7 +6253,7 @@
       <c r="B49" s="3">
         <v>45</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="16" t="s">
         <v>100</v>
       </c>
     </row>
@@ -6351,7 +6264,7 @@
       <c r="B50" s="3">
         <v>46</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="16" t="s">
         <v>72</v>
       </c>
     </row>
@@ -6362,7 +6275,7 @@
       <c r="B51" s="3">
         <v>47</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="16" t="s">
         <v>73</v>
       </c>
     </row>
@@ -6373,7 +6286,7 @@
       <c r="B52" s="3">
         <v>48</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="16" t="s">
         <v>74</v>
       </c>
     </row>
@@ -6384,7 +6297,7 @@
       <c r="B53" s="3">
         <v>49</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="16" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6395,7 +6308,7 @@
       <c r="B54" s="3">
         <v>50</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="16" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor code structure for improved readability and maintainability, added instructions, modified readme
</commit_message>
<xml_diff>
--- a/exercise_1_etl_pipeline/data/relaciones.xlsx
+++ b/exercise_1_etl_pipeline/data/relaciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugen\Desktop\Palace\the-palace-company-challenge\exercise_1_etl_pipeline\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diani\Dropbox\1 TESIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5619734E-C118-4909-9C10-13EC0CC3579A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC2D9E4-00E1-40C4-8CAD-4885B247E882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz de adyacencia" sheetId="1" r:id="rId1"/>
@@ -433,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -447,18 +447,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -742,13 +753,13 @@
   <dimension ref="A1:AZ52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
   </cols>
@@ -982,10 +993,10 @@
       <c r="AA2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AB2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AC2" s="9" t="s">
         <v>25</v>
       </c>
       <c r="AD2" s="1" t="s">
@@ -1065,154 +1076,154 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6">
-        <v>1</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0</v>
-      </c>
-      <c r="K3" s="8">
-        <v>0</v>
-      </c>
-      <c r="L3" s="6">
-        <v>1</v>
-      </c>
-      <c r="M3" s="8">
-        <v>0</v>
-      </c>
-      <c r="N3" s="8">
-        <v>0</v>
-      </c>
-      <c r="O3" s="8">
-        <v>0</v>
-      </c>
-      <c r="P3" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="8">
-        <v>0</v>
-      </c>
-      <c r="R3" s="8">
-        <v>0</v>
-      </c>
-      <c r="S3" s="8">
-        <v>0</v>
-      </c>
-      <c r="T3" s="8">
-        <v>0</v>
-      </c>
-      <c r="U3" s="8">
-        <v>0</v>
-      </c>
-      <c r="V3" s="8">
-        <v>0</v>
-      </c>
-      <c r="W3" s="9">
-        <v>0</v>
-      </c>
-      <c r="X3" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="6">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AH3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AI3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AJ3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AL3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AT3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AU3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AV3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AW3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AX3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AY3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AZ3" s="3">
+      <c r="C3" s="15">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0</v>
+      </c>
+      <c r="J3" s="10">
+        <v>0</v>
+      </c>
+      <c r="K3" s="10">
+        <v>0</v>
+      </c>
+      <c r="L3" s="7">
+        <v>1</v>
+      </c>
+      <c r="M3" s="10">
+        <v>0</v>
+      </c>
+      <c r="N3" s="10">
+        <v>0</v>
+      </c>
+      <c r="O3" s="10">
+        <v>0</v>
+      </c>
+      <c r="P3" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>0</v>
+      </c>
+      <c r="R3" s="10">
+        <v>0</v>
+      </c>
+      <c r="S3" s="10">
+        <v>0</v>
+      </c>
+      <c r="T3" s="10">
+        <v>0</v>
+      </c>
+      <c r="U3" s="10">
+        <v>0</v>
+      </c>
+      <c r="V3" s="10">
+        <v>0</v>
+      </c>
+      <c r="W3" s="11">
+        <v>0</v>
+      </c>
+      <c r="X3" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="12">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="13">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="13">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="13">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="13">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="13">
+        <v>1</v>
+      </c>
+      <c r="AL3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AW3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AX3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AY3" s="13">
+        <v>0</v>
+      </c>
+      <c r="AZ3" s="13">
         <v>0</v>
       </c>
     </row>
@@ -1226,7 +1237,7 @@
       <c r="C4" s="6">
         <v>0</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="15">
         <v>0</v>
       </c>
       <c r="E4" s="6">
@@ -1283,7 +1294,7 @@
       <c r="V4" s="3">
         <v>0</v>
       </c>
-      <c r="W4" s="7">
+      <c r="W4" s="8">
         <v>0</v>
       </c>
       <c r="X4" s="3">
@@ -1387,7 +1398,7 @@
       <c r="D5" s="6">
         <v>0</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="15">
         <v>0</v>
       </c>
       <c r="F5" s="6">
@@ -1441,7 +1452,7 @@
       <c r="V5" s="3">
         <v>0</v>
       </c>
-      <c r="W5" s="7">
+      <c r="W5" s="8">
         <v>0</v>
       </c>
       <c r="X5" s="3">
@@ -1548,7 +1559,7 @@
       <c r="E6" s="6">
         <v>1</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="15">
         <v>0</v>
       </c>
       <c r="G6" s="6">
@@ -1599,7 +1610,7 @@
       <c r="V6" s="3">
         <v>0</v>
       </c>
-      <c r="W6" s="7">
+      <c r="W6" s="8">
         <v>0</v>
       </c>
       <c r="X6" s="3">
@@ -1709,7 +1720,7 @@
       <c r="F7" s="6">
         <v>1</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="15">
         <v>0</v>
       </c>
       <c r="H7" s="6">
@@ -1757,7 +1768,7 @@
       <c r="V7" s="3">
         <v>0</v>
       </c>
-      <c r="W7" s="7">
+      <c r="W7" s="8">
         <v>0</v>
       </c>
       <c r="X7" s="3">
@@ -1870,7 +1881,7 @@
       <c r="G8" s="6">
         <v>1</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="15">
         <v>0</v>
       </c>
       <c r="I8" s="6">
@@ -1915,7 +1926,7 @@
       <c r="V8" s="3">
         <v>0</v>
       </c>
-      <c r="W8" s="7">
+      <c r="W8" s="8">
         <v>0</v>
       </c>
       <c r="X8" s="3">
@@ -2031,7 +2042,7 @@
       <c r="H9" s="6">
         <v>1</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="15">
         <v>0</v>
       </c>
       <c r="J9" s="3">
@@ -2073,7 +2084,7 @@
       <c r="V9" s="3">
         <v>0</v>
       </c>
-      <c r="W9" s="7">
+      <c r="W9" s="8">
         <v>0</v>
       </c>
       <c r="X9" s="3">
@@ -2192,7 +2203,7 @@
       <c r="I10" s="3">
         <v>1</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="15">
         <v>0</v>
       </c>
       <c r="K10" s="3">
@@ -2231,7 +2242,7 @@
       <c r="V10" s="3">
         <v>0</v>
       </c>
-      <c r="W10" s="7">
+      <c r="W10" s="8">
         <v>0</v>
       </c>
       <c r="X10" s="3">
@@ -2353,7 +2364,7 @@
       <c r="J11" s="3">
         <v>1</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="15">
         <v>0</v>
       </c>
       <c r="L11" s="3">
@@ -2389,7 +2400,7 @@
       <c r="V11" s="3">
         <v>0</v>
       </c>
-      <c r="W11" s="7">
+      <c r="W11" s="8">
         <v>0</v>
       </c>
       <c r="X11" s="3">
@@ -2514,7 +2525,7 @@
       <c r="K12" s="3">
         <v>1</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="15">
         <v>0</v>
       </c>
       <c r="M12" s="3">
@@ -2547,7 +2558,7 @@
       <c r="V12" s="3">
         <v>0</v>
       </c>
-      <c r="W12" s="7">
+      <c r="W12" s="8">
         <v>0</v>
       </c>
       <c r="X12" s="3">
@@ -2675,7 +2686,7 @@
       <c r="L13" s="3">
         <v>1</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="15">
         <v>0</v>
       </c>
       <c r="N13" s="3">
@@ -2705,7 +2716,7 @@
       <c r="V13" s="3">
         <v>0</v>
       </c>
-      <c r="W13" s="7">
+      <c r="W13" s="8">
         <v>0</v>
       </c>
       <c r="X13" s="3">
@@ -2836,7 +2847,7 @@
       <c r="M14" s="3">
         <v>1</v>
       </c>
-      <c r="N14" s="11">
+      <c r="N14" s="15">
         <v>0</v>
       </c>
       <c r="O14" s="3">
@@ -2863,7 +2874,7 @@
       <c r="V14" s="3">
         <v>0</v>
       </c>
-      <c r="W14" s="7">
+      <c r="W14" s="8">
         <v>0</v>
       </c>
       <c r="X14" s="3">
@@ -2997,7 +3008,7 @@
       <c r="N15" s="3">
         <v>0</v>
       </c>
-      <c r="O15" s="11">
+      <c r="O15" s="15">
         <v>0</v>
       </c>
       <c r="P15" s="3">
@@ -3021,7 +3032,7 @@
       <c r="V15" s="3">
         <v>0</v>
       </c>
-      <c r="W15" s="7">
+      <c r="W15" s="8">
         <v>0</v>
       </c>
       <c r="X15" s="3">
@@ -3158,7 +3169,7 @@
       <c r="O16" s="3">
         <v>1</v>
       </c>
-      <c r="P16" s="11">
+      <c r="P16" s="15">
         <v>0</v>
       </c>
       <c r="Q16" s="3">
@@ -3179,7 +3190,7 @@
       <c r="V16" s="3">
         <v>0</v>
       </c>
-      <c r="W16" s="7">
+      <c r="W16" s="8">
         <v>0</v>
       </c>
       <c r="X16" s="3">
@@ -3319,7 +3330,7 @@
       <c r="P17" s="3">
         <v>1</v>
       </c>
-      <c r="Q17" s="11">
+      <c r="Q17" s="15">
         <v>0</v>
       </c>
       <c r="R17" s="3">
@@ -3337,7 +3348,7 @@
       <c r="V17" s="3">
         <v>0</v>
       </c>
-      <c r="W17" s="7">
+      <c r="W17" s="8">
         <v>0</v>
       </c>
       <c r="X17" s="3">
@@ -3480,7 +3491,7 @@
       <c r="Q18" s="3">
         <v>1</v>
       </c>
-      <c r="R18" s="11">
+      <c r="R18" s="15">
         <v>0</v>
       </c>
       <c r="S18" s="3">
@@ -3495,7 +3506,7 @@
       <c r="V18" s="3">
         <v>1</v>
       </c>
-      <c r="W18" s="7">
+      <c r="W18" s="8">
         <v>1</v>
       </c>
       <c r="X18" s="3">
@@ -3641,7 +3652,7 @@
       <c r="R19" s="3">
         <v>1</v>
       </c>
-      <c r="S19" s="11">
+      <c r="S19" s="15">
         <v>0</v>
       </c>
       <c r="T19" s="3">
@@ -3653,7 +3664,7 @@
       <c r="V19" s="3">
         <v>1</v>
       </c>
-      <c r="W19" s="7">
+      <c r="W19" s="8">
         <v>1</v>
       </c>
       <c r="X19" s="3">
@@ -3751,156 +3762,58 @@
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="3">
-        <v>1</v>
-      </c>
-      <c r="D20" s="3">
-        <v>0</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0</v>
-      </c>
-      <c r="G20" s="3">
-        <v>0</v>
-      </c>
-      <c r="H20" s="3">
-        <v>0</v>
-      </c>
-      <c r="I20" s="3">
-        <v>0</v>
-      </c>
-      <c r="J20" s="3">
-        <v>0</v>
-      </c>
-      <c r="K20" s="3">
-        <v>0</v>
-      </c>
-      <c r="L20" s="3">
-        <v>0</v>
-      </c>
-      <c r="M20" s="3">
-        <v>0</v>
-      </c>
-      <c r="N20" s="3">
-        <v>0</v>
-      </c>
-      <c r="O20" s="3">
-        <v>0</v>
-      </c>
-      <c r="P20" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="3">
-        <v>0</v>
-      </c>
-      <c r="R20" s="3">
-        <v>0</v>
-      </c>
-      <c r="S20" s="3">
-        <v>0</v>
-      </c>
-      <c r="T20" s="11">
-        <v>0</v>
-      </c>
-      <c r="U20" s="3">
-        <v>0</v>
-      </c>
-      <c r="V20" s="3">
-        <v>0</v>
-      </c>
-      <c r="W20" s="7">
-        <v>0</v>
-      </c>
-      <c r="X20" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC20" s="7">
-        <v>0</v>
-      </c>
-      <c r="AD20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF20" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI20" s="7">
-        <v>0</v>
-      </c>
-      <c r="AJ20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AK20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL20" s="7">
-        <v>0</v>
-      </c>
-      <c r="AM20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AN20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AO20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AP20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AQ20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AR20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AS20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AT20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AU20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AV20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AW20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AX20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AY20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AZ20" s="3">
-        <v>0</v>
-      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="15">
+        <v>0</v>
+      </c>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="3"/>
+      <c r="AC20" s="3"/>
+      <c r="AD20" s="3"/>
+      <c r="AE20" s="3"/>
+      <c r="AF20" s="3"/>
+      <c r="AG20" s="3"/>
+      <c r="AH20" s="3"/>
+      <c r="AI20" s="3"/>
+      <c r="AJ20" s="3"/>
+      <c r="AK20" s="3"/>
+      <c r="AL20" s="3"/>
+      <c r="AM20" s="3"/>
+      <c r="AN20" s="3"/>
+      <c r="AO20" s="3"/>
+      <c r="AP20" s="3"/>
+      <c r="AQ20" s="3"/>
+      <c r="AR20" s="3"/>
+      <c r="AS20" s="3"/>
+      <c r="AT20" s="3"/>
+      <c r="AU20" s="3"/>
+      <c r="AV20" s="3"/>
+      <c r="AW20" s="3"/>
+      <c r="AX20" s="3"/>
+      <c r="AY20" s="3"/>
+      <c r="AZ20" s="3"/>
     </row>
     <row r="21" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
@@ -3927,11 +3840,11 @@
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
-      <c r="U21" s="11">
+      <c r="U21" s="15">
         <v>0</v>
       </c>
       <c r="V21" s="3"/>
-      <c r="W21" s="7"/>
+      <c r="W21" s="8"/>
       <c r="X21" s="3"/>
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
@@ -3988,10 +3901,10 @@
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
-      <c r="V22" s="11">
-        <v>0</v>
-      </c>
-      <c r="W22" s="7"/>
+      <c r="V22" s="15">
+        <v>0</v>
+      </c>
+      <c r="W22" s="8"/>
       <c r="X22" s="3"/>
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
@@ -4049,7 +3962,7 @@
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
-      <c r="W23" s="11">
+      <c r="W23" s="15">
         <v>0</v>
       </c>
       <c r="X23" s="3"/>
@@ -4109,8 +4022,8 @@
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
-      <c r="W24" s="7"/>
-      <c r="X24" s="11">
+      <c r="W24" s="8"/>
+      <c r="X24" s="15">
         <v>0</v>
       </c>
       <c r="Y24" s="3"/>
@@ -4169,9 +4082,9 @@
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
-      <c r="W25" s="7"/>
+      <c r="W25" s="8"/>
       <c r="X25" s="3"/>
-      <c r="Y25" s="11">
+      <c r="Y25" s="15">
         <v>0</v>
       </c>
       <c r="Z25" s="3"/>
@@ -4229,10 +4142,10 @@
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
-      <c r="W26" s="7"/>
+      <c r="W26" s="8"/>
       <c r="X26" s="3"/>
       <c r="Y26" s="3"/>
-      <c r="Z26" s="11">
+      <c r="Z26" s="15">
         <v>0</v>
       </c>
       <c r="AA26" s="3"/>
@@ -4289,11 +4202,11 @@
       <c r="T27" s="3"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
-      <c r="W27" s="7"/>
+      <c r="W27" s="8"/>
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
-      <c r="AA27" s="11">
+      <c r="AA27" s="15">
         <v>0</v>
       </c>
       <c r="AB27" s="3"/>
@@ -4323,7 +4236,7 @@
       <c r="AZ27" s="3"/>
     </row>
     <row r="28" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
+      <c r="A28" s="14">
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -4349,12 +4262,12 @@
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
-      <c r="W28" s="7"/>
+      <c r="W28" s="8"/>
       <c r="X28" s="3"/>
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
       <c r="AA28" s="3"/>
-      <c r="AB28" s="11">
+      <c r="AB28" s="15">
         <v>0</v>
       </c>
       <c r="AC28" s="3"/>
@@ -4415,7 +4328,7 @@
       <c r="Z29" s="3"/>
       <c r="AA29" s="3"/>
       <c r="AB29" s="3"/>
-      <c r="AC29" s="11">
+      <c r="AC29" s="15">
         <v>0</v>
       </c>
       <c r="AD29" s="3"/>
@@ -4476,7 +4389,7 @@
       <c r="AA30" s="3"/>
       <c r="AB30" s="3"/>
       <c r="AC30" s="3"/>
-      <c r="AD30" s="11">
+      <c r="AD30" s="15">
         <v>0</v>
       </c>
       <c r="AE30" s="3"/>
@@ -4537,7 +4450,7 @@
       <c r="AB31" s="3"/>
       <c r="AC31" s="3"/>
       <c r="AD31" s="3"/>
-      <c r="AE31" s="11">
+      <c r="AE31" s="15">
         <v>0</v>
       </c>
       <c r="AF31" s="3"/>
@@ -4598,7 +4511,7 @@
       <c r="AC32" s="3"/>
       <c r="AD32" s="3"/>
       <c r="AE32" s="3"/>
-      <c r="AF32" s="11">
+      <c r="AF32" s="15">
         <v>0</v>
       </c>
       <c r="AG32" s="3"/>
@@ -4659,7 +4572,7 @@
       <c r="AD33" s="3"/>
       <c r="AE33" s="3"/>
       <c r="AF33" s="3"/>
-      <c r="AG33" s="11">
+      <c r="AG33" s="15">
         <v>0</v>
       </c>
       <c r="AH33" s="3"/>
@@ -4720,7 +4633,7 @@
       <c r="AE34" s="3"/>
       <c r="AF34" s="3"/>
       <c r="AG34" s="3"/>
-      <c r="AH34" s="11">
+      <c r="AH34" s="15">
         <v>0</v>
       </c>
       <c r="AI34" s="3"/>
@@ -4781,7 +4694,7 @@
       <c r="AF35" s="3"/>
       <c r="AG35" s="3"/>
       <c r="AH35" s="3"/>
-      <c r="AI35" s="11">
+      <c r="AI35" s="15">
         <v>0</v>
       </c>
       <c r="AJ35" s="3"/>
@@ -4842,7 +4755,7 @@
       <c r="AG36" s="3"/>
       <c r="AH36" s="3"/>
       <c r="AI36" s="3"/>
-      <c r="AJ36" s="11">
+      <c r="AJ36" s="15">
         <v>0</v>
       </c>
       <c r="AK36" s="3"/>
@@ -4903,7 +4816,7 @@
       <c r="AH37" s="3"/>
       <c r="AI37" s="3"/>
       <c r="AJ37" s="3"/>
-      <c r="AK37" s="11">
+      <c r="AK37" s="15">
         <v>0</v>
       </c>
       <c r="AL37" s="3"/>
@@ -4964,7 +4877,7 @@
       <c r="AI38" s="3"/>
       <c r="AJ38" s="3"/>
       <c r="AK38" s="3"/>
-      <c r="AL38" s="11">
+      <c r="AL38" s="15">
         <v>0</v>
       </c>
       <c r="AM38" s="3"/>
@@ -5025,7 +4938,7 @@
       <c r="AJ39" s="3"/>
       <c r="AK39" s="3"/>
       <c r="AL39" s="3"/>
-      <c r="AM39" s="11">
+      <c r="AM39" s="15">
         <v>0</v>
       </c>
       <c r="AN39" s="3"/>
@@ -5086,7 +4999,7 @@
       <c r="AK40" s="3"/>
       <c r="AL40" s="3"/>
       <c r="AM40" s="3"/>
-      <c r="AN40" s="11">
+      <c r="AN40" s="15">
         <v>0</v>
       </c>
       <c r="AO40" s="3"/>
@@ -5147,7 +5060,7 @@
       <c r="AL41" s="3"/>
       <c r="AM41" s="3"/>
       <c r="AN41" s="3"/>
-      <c r="AO41" s="11">
+      <c r="AO41" s="15">
         <v>0</v>
       </c>
       <c r="AP41" s="3"/>
@@ -5208,7 +5121,7 @@
       <c r="AM42" s="3"/>
       <c r="AN42" s="3"/>
       <c r="AO42" s="3"/>
-      <c r="AP42" s="11">
+      <c r="AP42" s="15">
         <v>0</v>
       </c>
       <c r="AQ42" s="3"/>
@@ -5269,7 +5182,7 @@
       <c r="AN43" s="3"/>
       <c r="AO43" s="3"/>
       <c r="AP43" s="3"/>
-      <c r="AQ43" s="11">
+      <c r="AQ43" s="15">
         <v>0</v>
       </c>
       <c r="AR43" s="3"/>
@@ -5330,7 +5243,7 @@
       <c r="AO44" s="3"/>
       <c r="AP44" s="3"/>
       <c r="AQ44" s="3"/>
-      <c r="AR44" s="11">
+      <c r="AR44" s="15">
         <v>0</v>
       </c>
       <c r="AS44" s="3"/>
@@ -5391,7 +5304,7 @@
       <c r="AP45" s="3"/>
       <c r="AQ45" s="3"/>
       <c r="AR45" s="3"/>
-      <c r="AS45" s="11">
+      <c r="AS45" s="15">
         <v>0</v>
       </c>
       <c r="AT45" s="3"/>
@@ -5452,7 +5365,7 @@
       <c r="AQ46" s="3"/>
       <c r="AR46" s="3"/>
       <c r="AS46" s="3"/>
-      <c r="AT46" s="11">
+      <c r="AT46" s="15">
         <v>0</v>
       </c>
       <c r="AU46" s="3"/>
@@ -5513,7 +5426,7 @@
       <c r="AR47" s="3"/>
       <c r="AS47" s="3"/>
       <c r="AT47" s="3"/>
-      <c r="AU47" s="11">
+      <c r="AU47" s="15">
         <v>0</v>
       </c>
       <c r="AV47" s="3"/>
@@ -5574,7 +5487,7 @@
       <c r="AS48" s="3"/>
       <c r="AT48" s="3"/>
       <c r="AU48" s="3"/>
-      <c r="AV48" s="11">
+      <c r="AV48" s="15">
         <v>0</v>
       </c>
       <c r="AW48" s="3"/>
@@ -5635,7 +5548,7 @@
       <c r="AT49" s="3"/>
       <c r="AU49" s="3"/>
       <c r="AV49" s="3"/>
-      <c r="AW49" s="11">
+      <c r="AW49" s="15">
         <v>0</v>
       </c>
       <c r="AX49" s="3"/>
@@ -5696,7 +5609,7 @@
       <c r="AU50" s="3"/>
       <c r="AV50" s="3"/>
       <c r="AW50" s="3"/>
-      <c r="AX50" s="11">
+      <c r="AX50" s="15">
         <v>0</v>
       </c>
       <c r="AY50" s="3"/>
@@ -5757,7 +5670,7 @@
       <c r="AV51" s="3"/>
       <c r="AW51" s="3"/>
       <c r="AX51" s="3"/>
-      <c r="AY51" s="11">
+      <c r="AY51" s="15">
         <v>0</v>
       </c>
       <c r="AZ51" s="3"/>
@@ -5818,7 +5731,7 @@
       <c r="AW52" s="3"/>
       <c r="AX52" s="3"/>
       <c r="AY52" s="3"/>
-      <c r="AZ52" s="11">
+      <c r="AZ52" s="15">
         <v>0</v>
       </c>
     </row>
@@ -5836,7 +5749,7 @@
       <selection activeCell="C21" sqref="C21:C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.140625" customWidth="1"/>
@@ -5847,7 +5760,7 @@
       <c r="B4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="16"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -5856,7 +5769,7 @@
       <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="16" t="s">
         <v>29</v>
       </c>
     </row>
@@ -5867,7 +5780,7 @@
       <c r="B6" s="3">
         <v>2</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="16" t="s">
         <v>30</v>
       </c>
     </row>
@@ -5878,7 +5791,7 @@
       <c r="B7" s="3">
         <v>3</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="16" t="s">
         <v>31</v>
       </c>
     </row>
@@ -5889,7 +5802,7 @@
       <c r="B8" s="3">
         <v>4</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="16" t="s">
         <v>32</v>
       </c>
     </row>
@@ -5900,7 +5813,7 @@
       <c r="B9" s="3">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="16" t="s">
         <v>33</v>
       </c>
     </row>
@@ -5911,7 +5824,7 @@
       <c r="B10" s="3">
         <v>6</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="16" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5922,7 +5835,7 @@
       <c r="B11" s="3">
         <v>7</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="16" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5933,7 +5846,7 @@
       <c r="B12" s="3">
         <v>8</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="16" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5944,7 +5857,7 @@
       <c r="B13" s="3">
         <v>9</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="16" t="s">
         <v>37</v>
       </c>
     </row>
@@ -5955,7 +5868,7 @@
       <c r="B14" s="3">
         <v>10</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -5966,7 +5879,7 @@
       <c r="B15" s="3">
         <v>11</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="16" t="s">
         <v>39</v>
       </c>
     </row>
@@ -5977,7 +5890,7 @@
       <c r="B16" s="3">
         <v>12</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="16" t="s">
         <v>40</v>
       </c>
     </row>
@@ -5988,7 +5901,7 @@
       <c r="B17" s="3">
         <v>13</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="16" t="s">
         <v>41</v>
       </c>
     </row>
@@ -5999,7 +5912,7 @@
       <c r="B18" s="3">
         <v>14</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="17" t="s">
         <v>42</v>
       </c>
     </row>
@@ -6010,7 +5923,7 @@
       <c r="B19" s="3">
         <v>15</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="17" t="s">
         <v>43</v>
       </c>
     </row>
@@ -6021,7 +5934,7 @@
       <c r="B20" s="3">
         <v>16</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="17" t="s">
         <v>44</v>
       </c>
     </row>
@@ -6032,7 +5945,7 @@
       <c r="B21" s="3">
         <v>17</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="17" t="s">
         <v>45</v>
       </c>
     </row>
@@ -6043,7 +5956,7 @@
       <c r="B22" s="3">
         <v>18</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="17" t="s">
         <v>46</v>
       </c>
     </row>
@@ -6054,7 +5967,7 @@
       <c r="B23" s="3">
         <v>19</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="17" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6065,7 +5978,7 @@
       <c r="B24" s="3">
         <v>20</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="17" t="s">
         <v>48</v>
       </c>
     </row>
@@ -6076,7 +5989,7 @@
       <c r="B25" s="3">
         <v>21</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="17" t="s">
         <v>49</v>
       </c>
     </row>
@@ -6087,7 +6000,7 @@
       <c r="B26" s="3">
         <v>22</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -6098,7 +6011,7 @@
       <c r="B27" s="3">
         <v>23</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="17" t="s">
         <v>51</v>
       </c>
     </row>
@@ -6109,7 +6022,7 @@
       <c r="B28" s="3">
         <v>24</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -6120,7 +6033,7 @@
       <c r="B29" s="3">
         <v>25</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="16" t="s">
         <v>53</v>
       </c>
     </row>
@@ -6131,7 +6044,7 @@
       <c r="B30" s="3">
         <v>26</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="16" t="s">
         <v>54</v>
       </c>
     </row>
@@ -6142,7 +6055,7 @@
       <c r="B31" s="3">
         <v>27</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="16" t="s">
         <v>55</v>
       </c>
     </row>
@@ -6153,7 +6066,7 @@
       <c r="B32" s="3">
         <v>28</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="16" t="s">
         <v>99</v>
       </c>
     </row>
@@ -6164,7 +6077,7 @@
       <c r="B33" s="3">
         <v>29</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="16" t="s">
         <v>56</v>
       </c>
     </row>
@@ -6175,7 +6088,7 @@
       <c r="B34" s="3">
         <v>30</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="16" t="s">
         <v>57</v>
       </c>
     </row>
@@ -6186,7 +6099,7 @@
       <c r="B35" s="3">
         <v>31</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="16" t="s">
         <v>58</v>
       </c>
     </row>
@@ -6197,7 +6110,7 @@
       <c r="B36" s="3">
         <v>32</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="16" t="s">
         <v>59</v>
       </c>
     </row>
@@ -6208,7 +6121,7 @@
       <c r="B37" s="3">
         <v>33</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="16" t="s">
         <v>60</v>
       </c>
     </row>
@@ -6219,7 +6132,7 @@
       <c r="B38" s="3">
         <v>34</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="16" t="s">
         <v>61</v>
       </c>
     </row>
@@ -6230,7 +6143,7 @@
       <c r="B39" s="3">
         <v>35</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="16" t="s">
         <v>62</v>
       </c>
     </row>
@@ -6241,7 +6154,7 @@
       <c r="B40" s="3">
         <v>36</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="16" t="s">
         <v>63</v>
       </c>
     </row>
@@ -6252,7 +6165,7 @@
       <c r="B41" s="3">
         <v>37</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="16" t="s">
         <v>64</v>
       </c>
     </row>
@@ -6263,7 +6176,7 @@
       <c r="B42" s="3">
         <v>38</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="16" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6274,7 +6187,7 @@
       <c r="B43" s="3">
         <v>39</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="16" t="s">
         <v>66</v>
       </c>
     </row>
@@ -6285,7 +6198,7 @@
       <c r="B44" s="3">
         <v>40</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="16" t="s">
         <v>67</v>
       </c>
     </row>
@@ -6296,7 +6209,7 @@
       <c r="B45" s="3">
         <v>41</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="16" t="s">
         <v>68</v>
       </c>
     </row>
@@ -6307,7 +6220,7 @@
       <c r="B46" s="3">
         <v>42</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="16" t="s">
         <v>69</v>
       </c>
     </row>
@@ -6318,7 +6231,7 @@
       <c r="B47" s="3">
         <v>43</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="16" t="s">
         <v>70</v>
       </c>
     </row>
@@ -6329,7 +6242,7 @@
       <c r="B48" s="3">
         <v>44</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="16" t="s">
         <v>71</v>
       </c>
     </row>
@@ -6340,7 +6253,7 @@
       <c r="B49" s="3">
         <v>45</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="16" t="s">
         <v>100</v>
       </c>
     </row>
@@ -6351,7 +6264,7 @@
       <c r="B50" s="3">
         <v>46</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="16" t="s">
         <v>72</v>
       </c>
     </row>
@@ -6362,7 +6275,7 @@
       <c r="B51" s="3">
         <v>47</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="16" t="s">
         <v>73</v>
       </c>
     </row>
@@ -6373,7 +6286,7 @@
       <c r="B52" s="3">
         <v>48</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="16" t="s">
         <v>74</v>
       </c>
     </row>
@@ -6384,7 +6297,7 @@
       <c r="B53" s="3">
         <v>49</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="16" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6395,7 +6308,7 @@
       <c r="B54" s="3">
         <v>50</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="16" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>